<commit_message>
Read From Document and Create Values in DB missing errorproof
</commit_message>
<xml_diff>
--- a/doc/FormatoDemo.xlsx
+++ b/doc/FormatoDemo.xlsx
@@ -5,214 +5,263 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="REGISTRO QUITO" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="REGISTRO PORTOVIEJO" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="60">
-  <si>
-    <t>PROGRAMA HABLAME DE TI</t>
-  </si>
-  <si>
-    <t>FUNDACION CECILIA RIVADENEIRA      
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
+  <si>
+    <t xml:space="preserve">PROGRAMA HABLAME DE TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNDACION CECILIA RIVADENEIRA      
 PROGRAMA DE INVESTIGACIÓN HABLAME DE TI</t>
   </si>
   <si>
-    <t>REGISTRO 2015 QUITO</t>
-  </si>
-  <si>
-    <t>Nº ENCUESTA</t>
-  </si>
-  <si>
-    <t>HOSPITAL</t>
-  </si>
-  <si>
-    <t>FECHA ENCUESTA (dd7mm/aa)</t>
-  </si>
-  <si>
-    <t>NOMBRE COMPLETO</t>
-  </si>
-  <si>
-    <t>FECHA DE NACIMIENTO</t>
-  </si>
-  <si>
-    <t>DIRECCION DOMICILIO</t>
-  </si>
-  <si>
-    <t>CIUDAD O PROV.</t>
-  </si>
-  <si>
-    <t>TELEFONO FIJO</t>
-  </si>
-  <si>
-    <t>CELULAR</t>
-  </si>
-  <si>
-    <t>NOMBRE MAMÁ O TUTOR</t>
-  </si>
-  <si>
-    <t>CORREO ELECTRONICO / FB</t>
-  </si>
-  <si>
-    <t>DIAGNOSTICO</t>
-  </si>
-  <si>
-    <t>FECHA INICIO TRATAMIENTO</t>
-  </si>
-  <si>
-    <t>OBSERVACION FAMILIAS</t>
-  </si>
-  <si>
-    <t>SUEÑO DEL NIÑ@</t>
-  </si>
-  <si>
-    <t>BENEFICIARIO DE (Bonos/Fundaciones)</t>
-  </si>
-  <si>
-    <t>INTERESADO EN (Programas de la FCR)</t>
-  </si>
-  <si>
-    <t>ENCUESTA realizada si/no</t>
-  </si>
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>Baca Ortiz</t>
-  </si>
-  <si>
-    <t>LEUCEMIA LLA</t>
-  </si>
-  <si>
-    <t>falta encuesta niño.</t>
-  </si>
-  <si>
-    <t>Baca Ortiz-ASONIC</t>
-  </si>
-  <si>
-    <t>–</t>
-  </si>
-  <si>
-    <t>Estable.</t>
-  </si>
-  <si>
-    <t>Metropolitano</t>
-  </si>
-  <si>
-    <t>En tratamiento</t>
-  </si>
-  <si>
-    <t>Solca</t>
-  </si>
-  <si>
-    <t>Eugenio Espejo</t>
-  </si>
-  <si>
-    <t>RETINOBLASTOMA</t>
-  </si>
-  <si>
-    <t>Hospital Militar</t>
-  </si>
-  <si>
-    <t>OSTEOSARCOMA 2do. Grado</t>
-  </si>
-  <si>
-    <t>SOLCA-CUENCA</t>
-  </si>
-  <si>
-    <t>LEUCEMIA LMA</t>
-  </si>
-  <si>
-    <t>LEUCEMIA LLA tipo B</t>
-  </si>
-  <si>
-    <t>TUMOR DE WILMS (nefroblastoma-tumor de riñón)</t>
-  </si>
-  <si>
-    <t>Trombosis escencial</t>
-  </si>
-  <si>
-    <t>EN tratameinto.</t>
-  </si>
-  <si>
-    <t>PROGRAMA DE INVESTIGACIÓN HABLAME DE TI</t>
-  </si>
-  <si>
-    <t>REGISTRO 2015 PORTOVIEJO</t>
-  </si>
-  <si>
-    <t>FECHA ENCUESTA (mm/dd/aa)</t>
-  </si>
-  <si>
-    <t>FECHA DE NACIMIENTO (mm/dd/aa)</t>
-  </si>
-  <si>
-    <t>SOLCA</t>
-  </si>
-  <si>
-    <t>PORTOVIEJO / MANABI</t>
-  </si>
-  <si>
-    <t>LEUCEMIA LINFOBLASTICA AGUDA</t>
-  </si>
-  <si>
-    <t>en tratamiento</t>
-  </si>
-  <si>
-    <t>CHONE / MANABI</t>
-  </si>
-  <si>
-    <t>OSTEOSARCOMA</t>
-  </si>
-  <si>
-    <t>MANTENIMIENTO</t>
-  </si>
-  <si>
-    <t>GUAYAS</t>
-  </si>
-  <si>
-    <t>MANABI</t>
-  </si>
-  <si>
-    <t>MANTA / MANABI</t>
-  </si>
-  <si>
-    <t>en tratamiento fase mantenimiento</t>
-  </si>
-  <si>
-    <t>RABDIOSARCOMA DE OJO DERECHO</t>
-  </si>
-  <si>
-    <t>CHONE MANABI</t>
-  </si>
-  <si>
-    <t>MANTA</t>
-  </si>
-  <si>
-    <t>PORTOVIEJO</t>
+    <t xml:space="preserve">REGISTRO 2015 QUITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nº ENCUESTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOSPITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA ENCUESTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE COMPLETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA DE NACIMIENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECCION DOMICILIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIUDAD O PROV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELEFONO FIJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELULAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE MAMÁ O TUTOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORREO ELECTRONICO / FB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIAGNOSTICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA INICIO TRATAMIENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBSERVACION FAMILIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUEÑO DEL NIÑ@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENEFICIARIO DE (Bonos/Fundaciones)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTERESADO EN (Programas de la FCR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENCUESTA realizada si/no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baca Ortiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29/02/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nino 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direccion 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEUCEMIA LLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sueno 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falta encuesta niño.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baca Ortiz-ASONIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/08/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nino 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direccion 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guayaquil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sueno 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">–</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metropolitano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/01/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nino 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direecion 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sueno 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tratamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/01/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nino 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direccion 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sueno 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hospital Baca Ortiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/01/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mateo Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEUCEMIA LINFOBLASTICA AGUDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">viajar a la playa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROGRAMA DE INVESTIGACIÓN HABLAME DE TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGISTRO 2015 PORTOVIEJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA ENCUESTA (mm/dd/aa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FECHA DE NACIMIENTO (mm/dd/aa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOLCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORTOVIEJO / MANABI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en tratamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHONE / MANABI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSTEOSARCOMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANTENIMIENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUAYAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANABI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANTA / MANABI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en tratamiento fase mantenimiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RABDIOSARCOMA DE OJO DERECHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHONE MANABI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORTOVIEJO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="MMM\-YY"/>
+    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="167" formatCode="MMM\-YY"/>
   </numFmts>
   <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -287,15 +336,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="12"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="12"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -350,14 +399,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor rgb="FF9999FF"/>
+        <fgColor rgb="FFCCC0D9"/>
+        <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCC0D9"/>
-        <bgColor rgb="FFD8D8D8"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FF9999FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -415,7 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -476,6 +525,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -496,51 +553,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,11 +641,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -724,14 +777,27 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="17" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3112244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.6530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.1785714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.4795918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.6428571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="37.6530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="42.234693877551"/>
     <col collapsed="false" hidden="true" max="18" min="18" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,33 +1015,45 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="C9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="15" t="n">
+        <v>37663</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M9" s="14"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="O9" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="17"/>
+      <c r="R9" s="19"/>
       <c r="S9" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,30 +1061,42 @@
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="15" t="n">
+        <v>37664</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M10" s="14"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="4"/>
+      <c r="O10" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="R10" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="R10" s="20"/>
       <c r="S10" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,348 +1104,322 @@
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="15" t="n">
+        <v>37665</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M11" s="4"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="4"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" s="20"/>
+      <c r="S11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="15" t="n">
+        <v>37666</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="R11" s="18"/>
-      <c r="S11" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="4"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="M12" s="14"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="O12" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="R12" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="R12" s="20"/>
       <c r="S12" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="11"/>
+      <c r="B13" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <v>37667</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="17"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
       <c r="S13" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="n">
-        <v>6</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="A14" s="13"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="13"/>
       <c r="I14" s="11"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="4"/>
       <c r="M14" s="14"/>
       <c r="N14" s="11"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="11"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="R14" s="20"/>
+      <c r="S14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="4"/>
       <c r="M15" s="14"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="17"/>
-      <c r="S15" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="B16" s="17"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="14"/>
       <c r="D16" s="4"/>
       <c r="E16" s="14"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="23"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="L16" s="4"/>
       <c r="M16" s="14"/>
       <c r="N16" s="11"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="11"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="R16" s="19"/>
+      <c r="S16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="n">
-        <v>9</v>
-      </c>
-      <c r="B17" s="25"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="26"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="K17" s="23"/>
+      <c r="L17" s="4"/>
       <c r="M17" s="14"/>
       <c r="N17" s="11"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="54.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="25"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="n">
-        <v>10</v>
-      </c>
+      <c r="A19" s="28"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="4"/>
       <c r="K19" s="11"/>
-      <c r="L19" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="L19" s="4"/>
       <c r="M19" s="13"/>
       <c r="N19" s="11"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="11"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
-        <v>11</v>
-      </c>
+      <c r="R19" s="19"/>
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="21"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4"/>
       <c r="I20" s="11"/>
       <c r="J20" s="4"/>
       <c r="K20" s="11"/>
-      <c r="L20" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="L20" s="11"/>
       <c r="M20" s="14"/>
-      <c r="N20" s="29"/>
+      <c r="N20" s="30"/>
       <c r="O20" s="11"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="11"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="R20" s="19"/>
+      <c r="S20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="n">
-        <v>12</v>
-      </c>
+      <c r="A21" s="13"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="28"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
       <c r="K21" s="11"/>
-      <c r="L21" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21" s="28"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
       <c r="S21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="n">
-        <v>13</v>
-      </c>
+      <c r="A22" s="13"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="21"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="4"/>
       <c r="E22" s="14"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="18"/>
       <c r="I22" s="11"/>
       <c r="J22" s="4"/>
       <c r="K22" s="11"/>
-      <c r="L22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="21"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="29"/>
       <c r="N22" s="11"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="11"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="R22" s="19"/>
+      <c r="S22" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="4">
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A6:S6"/>
     <mergeCell ref="A7:T7"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1374,109 +1438,112 @@
   </sheetPr>
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.1479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="8" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="54.7448979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.8367346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="50.4336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="42.3775510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="31.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="44.3214285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.3469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.280612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.9132653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -1497,11 +1564,11 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-      <c r="S5" s="31"/>
+      <c r="S5" s="32"/>
     </row>
     <row r="6" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1520,11 +1587,11 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="S6" s="31"/>
+      <c r="S6" s="32"/>
     </row>
     <row r="7" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1549,529 +1616,529 @@
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="32" t="s">
+      <c r="E8" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="32" t="s">
+      <c r="L8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="32" t="s">
+      <c r="O8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="P8" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="34" t="s">
+      <c r="Q8" s="35" t="s">
         <v>19</v>
       </c>
       <c r="R8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="S8" s="28"/>
+      <c r="S8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="4"/>
       <c r="E9" s="14"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="35"/>
+      <c r="K9" s="36"/>
       <c r="L9" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M9" s="14"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="36"/>
+      <c r="O9" s="37"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S9" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="S9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="4"/>
       <c r="E10" s="14"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M10" s="14"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="36"/>
+      <c r="O10" s="37"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S10" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="S10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="n">
+      <c r="A11" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="42"/>
+      <c r="B11" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="39"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="43"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="4"/>
       <c r="E12" s="14"/>
       <c r="F12" s="11"/>
       <c r="G12" s="4" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="M12" s="14"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="36"/>
+      <c r="O12" s="37"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S12" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="S12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="43"/>
+        <v>60</v>
+      </c>
+      <c r="C13" s="44"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="21"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="11"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="35"/>
+      <c r="K13" s="36"/>
       <c r="L13" s="11" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="M13" s="14"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="36"/>
+      <c r="O13" s="37"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S13" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="S13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="n">
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="4"/>
       <c r="E14" s="14"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="11"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="35"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M14" s="14"/>
       <c r="N14" s="11"/>
-      <c r="O14" s="36"/>
+      <c r="O14" s="37"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S14" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="S14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="n">
+      <c r="A15" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="17" t="s">
+      <c r="B15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="45"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M15" s="45"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="S15" s="42"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="S15" s="43"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="n">
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="4"/>
       <c r="E16" s="14"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="23"/>
+        <v>68</v>
+      </c>
+      <c r="H16" s="24"/>
       <c r="I16" s="11"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="35"/>
+      <c r="K16" s="36"/>
       <c r="L16" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M16" s="14"/>
       <c r="N16" s="11"/>
-      <c r="O16" s="36"/>
+      <c r="O16" s="37"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S16" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="S16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="n">
+      <c r="A17" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>45</v>
+      <c r="B17" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="C17" s="26"/>
-      <c r="D17" s="25"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="26"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="M17" s="14"/>
       <c r="N17" s="11"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="S17" s="15"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="S17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="43"/>
+        <v>60</v>
+      </c>
+      <c r="C19" s="44"/>
       <c r="D19" s="4"/>
       <c r="E19" s="14"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="49"/>
+      <c r="K19" s="50"/>
       <c r="L19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M19" s="21"/>
+        <v>54</v>
+      </c>
+      <c r="M19" s="29"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="50"/>
+      <c r="O19" s="51"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S19" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="S19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="n">
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="43"/>
+        <v>60</v>
+      </c>
+      <c r="C20" s="44"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="21"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="11"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="49"/>
+      <c r="K20" s="50"/>
       <c r="L20" s="11" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M20" s="14"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="36"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="37"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S20" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="S20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="52"/>
+      <c r="E21" s="53"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="M21" s="52"/>
+      <c r="G21" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="M21" s="53"/>
       <c r="N21" s="11"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
       <c r="R21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S21" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="S21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="55"/>
+      <c r="E22" s="56"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="11"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="56"/>
+      <c r="K22" s="57"/>
       <c r="L22" s="4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="M22" s="14"/>
       <c r="N22" s="11"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="11"/>
-      <c r="R22" s="18"/>
+      <c r="R22" s="20"/>
       <c r="S22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="55"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M23" s="55"/>
+        <v>54</v>
+      </c>
+      <c r="M23" s="56"/>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
-      <c r="R23" s="18"/>
+      <c r="R23" s="20"/>
       <c r="S23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
       <c r="B24" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="55"/>
+      <c r="E24" s="56"/>
       <c r="F24" s="4"/>
       <c r="G24" s="11" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M24" s="55"/>
+        <v>54</v>
+      </c>
+      <c r="M24" s="56"/>
       <c r="N24" s="11"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="11"/>
-      <c r="R24" s="18"/>
+      <c r="R24" s="20"/>
       <c r="S24" s="4"/>
     </row>
   </sheetData>
@@ -2091,7 +2158,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Change Documents to Originals and Erase Extra Documents
</commit_message>
<xml_diff>
--- a/doc/FormatoDemo.xlsx
+++ b/doc/FormatoDemo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="73">
   <si>
     <t xml:space="preserve">PROGRAMA HABLAME DE TI</t>
   </si>
@@ -39,13 +39,13 @@
     <t xml:space="preserve">HOSPITAL</t>
   </si>
   <si>
-    <t xml:space="preserve">FECHA ENCUESTA</t>
+    <t xml:space="preserve">FECHA ENCUESTA (mm/dd/aa)</t>
   </si>
   <si>
     <t xml:space="preserve">NOMBRE COMPLETO</t>
   </si>
   <si>
-    <t xml:space="preserve">FECHA DE NACIMIENTO</t>
+    <t xml:space="preserve">FECHA DE NACIMIENTO (mm/dd/aa)</t>
   </si>
   <si>
     <t xml:space="preserve">DIRECCION DOMICILIO</t>
@@ -199,12 +199,6 @@
   </si>
   <si>
     <t xml:space="preserve">REGISTRO 2015 PORTOVIEJO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FECHA ENCUESTA (mm/dd/aa)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FECHA DE NACIMIENTO (mm/dd/aa)</t>
   </si>
   <si>
     <t xml:space="preserve">SOLCA</t>
@@ -259,7 +253,7 @@
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="167" formatCode="MMM\-YY"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -324,6 +318,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -467,7 +468,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -504,11 +505,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -536,7 +541,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -556,14 +561,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -592,111 +597,111 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -779,28 +784,32 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3112244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.6530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.1785714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.4795918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.6428571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="37.6530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="42.234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.4744897959184"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.2857142857143"/>
     <col collapsed="false" hidden="true" max="18" min="18" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,7 +944,7 @@
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="27.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -959,7 +968,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
@@ -996,7 +1005,7 @@
       <c r="L8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="N8" s="8" t="s">
@@ -1005,80 +1014,80 @@
       <c r="O8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="P8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="R8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="S8" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
+      <c r="A9" s="14" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="15" t="n">
+      <c r="E9" s="16" t="n">
         <v>37663</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11" t="s">
+      <c r="M9" s="15"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
-      <c r="R9" s="19"/>
+      <c r="R9" s="20"/>
       <c r="S9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="14" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="15" t="n">
+      <c r="E10" s="16" t="n">
         <v>37664</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="17" t="s">
         <v>34</v>
       </c>
       <c r="H10" s="4"/>
@@ -1088,40 +1097,40 @@
       <c r="L10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="11"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="12"/>
       <c r="O10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="P10" s="4"/>
-      <c r="Q10" s="11" t="s">
+      <c r="Q10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R10" s="20"/>
+      <c r="R10" s="21"/>
       <c r="S10" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="14" t="n">
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="15" t="n">
+      <c r="E11" s="16" t="n">
         <v>37665</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="17" t="s">
         <v>42</v>
       </c>
       <c r="H11" s="4"/>
@@ -1132,297 +1141,297 @@
         <v>27</v>
       </c>
       <c r="M11" s="4"/>
-      <c r="N11" s="21"/>
+      <c r="N11" s="22"/>
       <c r="O11" s="4" t="s">
         <v>43</v>
       </c>
       <c r="P11" s="4"/>
-      <c r="Q11" s="11" t="s">
+      <c r="Q11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="20"/>
+      <c r="R11" s="21"/>
       <c r="S11" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="14" t="n">
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="15" t="n">
+      <c r="E12" s="16" t="n">
         <v>37666</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11" t="s">
+      <c r="M12" s="15"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12" t="s">
         <v>49</v>
       </c>
       <c r="P12" s="4"/>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="R12" s="20"/>
+      <c r="R12" s="21"/>
       <c r="S12" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="15" t="n">
+      <c r="E13" s="16" t="n">
         <v>37667</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="22" t="s">
+      <c r="K13" s="24"/>
+      <c r="L13" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22" t="s">
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
       <c r="S13" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="14" t="n">
         <v>6</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="11"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="23"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="11"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="12"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="20"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="21"/>
       <c r="S14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="16"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="23"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="19"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="20"/>
       <c r="S15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="14"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="25"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="11"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="12"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="19"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="20"/>
       <c r="S16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="26"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="27"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="23"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="11"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="12"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
       <c r="S17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="54.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
       <c r="S18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="11"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="11"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="12"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="19"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="20"/>
       <c r="S19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="29"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="16"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="11"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="11"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="12"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="19"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="20"/>
       <c r="S20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="22"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
       <c r="S21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="29"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="11"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="11"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="11"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="12"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="19"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="20"/>
       <c r="S22" s="4"/>
     </row>
   </sheetData>
@@ -1450,111 +1459,115 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.7857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.9795918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.1224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="44.3214285714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="38.3469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.280612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.4795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="59.9387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="52.780612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="48.7295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -1575,7 +1588,7 @@
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
-      <c r="S5" s="32"/>
+      <c r="S5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
@@ -1598,7 +1611,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="S6" s="32"/>
+      <c r="S6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
@@ -1627,103 +1640,103 @@
       <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="S8" s="23"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="P8" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="S8" s="22"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="36"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="37"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="38"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S9" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="S9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="14" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1732,383 +1745,383 @@
       <c r="L10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="37"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="38"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="12"/>
       <c r="R10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S10" s="18"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M11" s="40"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="44"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="S10" s="17"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19" t="s">
+      <c r="M12" s="15"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" s="39"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="43"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M12" s="14"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" s="17"/>
+      <c r="S12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="14" t="n">
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="44"/>
+        <v>59</v>
+      </c>
+      <c r="C13" s="45"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" s="14"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="11"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M13" s="15"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="12"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S13" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="S13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="14" t="n">
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="14"/>
+      <c r="E14" s="15"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="13"/>
-      <c r="I14" s="11"/>
+        <v>66</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="36"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="37"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="38"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="11"/>
+      <c r="Q14" s="12"/>
       <c r="R14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S14" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="S14" s="18"/>
     </row>
     <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="n">
+      <c r="A15" s="39" t="n">
         <v>7</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="19" t="s">
+      <c r="B15" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="M15" s="46"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="47"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="S15" s="43"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="S15" s="44"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="14" t="n">
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="C16" s="15"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="36"/>
+      <c r="K16" s="37"/>
       <c r="L16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="37"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="38"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="11"/>
+      <c r="Q16" s="12"/>
       <c r="R16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="S16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="n">
+      <c r="A17" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
+      <c r="B17" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
       <c r="L17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M17" s="14"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="S17" s="17"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="n">
+      <c r="A19" s="14" t="n">
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="44"/>
+        <v>59</v>
+      </c>
+      <c r="C19" s="45"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="14"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="50"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="29"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="51"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="52"/>
       <c r="P19" s="4"/>
-      <c r="Q19" s="11"/>
+      <c r="Q19" s="12"/>
       <c r="R19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S19" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="S19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="14" t="n">
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="44"/>
+        <v>59</v>
+      </c>
+      <c r="C20" s="45"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="29"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="15"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="M20" s="14"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S20" s="17"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="M21" s="54"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="53"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="17"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S21" s="17"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="C22" s="15"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="56"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="11"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="57"/>
+      <c r="K22" s="58"/>
       <c r="L22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M22" s="14"/>
-      <c r="N22" s="11"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="12"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="20"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="21"/>
       <c r="S22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="C23" s="15"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="56"/>
+      <c r="E23" s="57"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -2117,25 +2130,25 @@
       <c r="L23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="56"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="20"/>
+      <c r="M23" s="57"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="21"/>
       <c r="S23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="14"/>
+        <v>59</v>
+      </c>
+      <c r="C24" s="15"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="56"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="11" t="s">
-        <v>74</v>
+      <c r="G24" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -2144,12 +2157,12 @@
       <c r="L24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="56"/>
-      <c r="N24" s="11"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="12"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="20"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="21"/>
       <c r="S24" s="4"/>
     </row>
   </sheetData>

</xml_diff>